<commit_message>
Upload File added Service
</commit_message>
<xml_diff>
--- a/TaskSoliq/wwwroot/ReceivedReports/Employees.xlsx
+++ b/TaskSoliq/wwwroot/ReceivedReports/Employees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dotnetbillioner\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD5AC25-980F-47CC-9E06-FF79BFC2D8FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1431FC-BF6F-44A5-9E5A-A358F390BBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{598F896C-A960-4F77-9D97-4D3AC01573FC}"/>
   </bookViews>
@@ -42,34 +42,34 @@
     <t>LastName</t>
   </si>
   <si>
-    <t>Shazamhon</t>
-  </si>
-  <si>
-    <t>Karimova</t>
-  </si>
-  <si>
-    <t>Jazmanoy</t>
-  </si>
-  <si>
-    <t>Hoshimova</t>
-  </si>
-  <si>
-    <t>Jononbek</t>
-  </si>
-  <si>
-    <t>Gadoyev</t>
-  </si>
-  <si>
-    <t>Kumsanoy</t>
-  </si>
-  <si>
-    <t>Keldiyeva</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
     <t>EmployeeCategory</t>
+  </si>
+  <si>
+    <t>Javlon</t>
+  </si>
+  <si>
+    <t>Fayziyev</t>
+  </si>
+  <si>
+    <t>Qosimjon</t>
+  </si>
+  <si>
+    <t>Berdiyev</t>
+  </si>
+  <si>
+    <t>Farangiz</t>
+  </si>
+  <si>
+    <t>Muhammad Rizo</t>
+  </si>
+  <si>
+    <t>Keldiyev</t>
+  </si>
+  <si>
+    <t>Gadoyeva</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,66 +443,66 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>22</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>19</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>18</v>
       </c>
       <c r="D5">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>